<commit_message>
updated finished 6th q
</commit_message>
<xml_diff>
--- a/metro_budget_exercise.xlsx
+++ b/metro_budget_exercise.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aaron\Documents\DA8\Projects\budget_lookups-CaitlinC91\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{489B955E-22C1-4249-BAC6-3E60F5D741DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADE2241B-E046-411F-92B6-B27BF3E3B342}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="91">
   <si>
     <t>Department</t>
   </si>
@@ -304,6 +304,9 @@
   </si>
   <si>
     <t>Actual spending amount - budget amount for fiscal year 2019</t>
+  </si>
+  <si>
+    <t>BONUS VERSION</t>
   </si>
 </sst>
 </file>
@@ -462,7 +465,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -648,6 +651,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -809,7 +818,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -821,6 +830,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -877,6 +887,987 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>metro_budget!$B$81:$B$83</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Question 6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Department</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Budget</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>metro_budget!$A$84:$A$86</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>FY17</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FY18</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>FY19</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>metro_budget!$B$84:$B$86</c:f>
+              <c:numCache>
+                <c:formatCode>_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>24332100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24497400</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>24323000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2942-42D9-99FE-39998C5663A2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>metro_budget!$C$81:$C$83</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Question 6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Department</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Actual</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>metro_budget!$A$84:$A$86</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>FY17</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FY18</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>FY19</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>metro_budget!$C$84:$C$86</c:f>
+              <c:numCache>
+                <c:formatCode>_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>22408587.5499999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22655993.629999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>23434073.089999899</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-2942-42D9-99FE-39998C5663A2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="182"/>
+        <c:axId val="1409884559"/>
+        <c:axId val="1409886223"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1409884559"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1409886223"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1409886223"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1409884559"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1285875</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E68835DA-C350-C113-B34A-7629F0896F63}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1178,8 +2169,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="D86" sqref="D86"/>
+    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="A83" sqref="A83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1284,7 +2275,7 @@
         <v>-9.4972027086493035E-2</v>
       </c>
       <c r="K2">
-        <f>RANK(J2,J:J,1)</f>
+        <f>_xlfn.RANK.EQ(J2,$J$2:$J$52,1)</f>
         <v>10</v>
       </c>
       <c r="L2">
@@ -1343,7 +2334,7 @@
         <v>-6.6804928315415249E-2</v>
       </c>
       <c r="K3">
-        <f t="shared" ref="K3:K52" si="5">RANK(J3,J:J,1)</f>
+        <f t="shared" ref="K3:K52" si="5">_xlfn.RANK.EQ(J3,$J$2:$J$52,1)</f>
         <v>14</v>
       </c>
       <c r="L3">
@@ -4260,6 +5251,12 @@
       <c r="A54" s="2" t="s">
         <v>67</v>
       </c>
+      <c r="F54" t="s">
+        <v>90</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
@@ -4272,6 +5269,18 @@
         <v>8</v>
       </c>
       <c r="D55" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G55" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="H55" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="I55" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="J55" s="9" t="s">
         <v>13</v>
       </c>
     </row>
@@ -4291,6 +5300,9 @@
         <f>VLOOKUP(A56,A2:N52,14, FALSE)</f>
         <v>-9181.0800000000163</v>
       </c>
+      <c r="G56" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
@@ -4308,6 +5320,9 @@
         <f t="shared" ref="D57:D61" si="11">VLOOKUP(A57,A3:N53,14, FALSE)</f>
         <v>-311228.08999999997</v>
       </c>
+      <c r="G57" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
@@ -4325,6 +5340,9 @@
         <f t="shared" si="11"/>
         <v>-374962.91000000015</v>
       </c>
+      <c r="G58" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
@@ -4342,6 +5360,9 @@
         <f t="shared" si="11"/>
         <v>-72.879999999888241</v>
       </c>
+      <c r="G59" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
@@ -4359,6 +5380,9 @@
         <f t="shared" si="11"/>
         <v>-1724.9000000000233</v>
       </c>
+      <c r="G60" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
@@ -4376,11 +5400,17 @@
         <f t="shared" si="11"/>
         <v>-82077.349999999627</v>
       </c>
+      <c r="G61" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
         <v>68</v>
       </c>
+      <c r="G63" s="7" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
@@ -4395,8 +5425,20 @@
       <c r="D64" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G64" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="H64" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="I64" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="J64" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>24</v>
       </c>
@@ -4412,8 +5454,11 @@
         <f>_xlfn.XLOOKUP(A65,A2:A52,N2:N52)</f>
         <v>-9181.0800000000163</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G65" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>25</v>
       </c>
@@ -4429,8 +5474,11 @@
         <f t="shared" ref="D66:D70" si="14">_xlfn.XLOOKUP(A66,A3:A53,N3:N53)</f>
         <v>-311228.08999999997</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G66" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>32</v>
       </c>
@@ -4446,8 +5494,11 @@
         <f t="shared" si="14"/>
         <v>-374962.91000000015</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G67" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>38</v>
       </c>
@@ -4463,8 +5514,11 @@
         <f t="shared" si="14"/>
         <v>-72.879999999888241</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G68" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>39</v>
       </c>
@@ -4480,8 +5534,11 @@
         <f t="shared" si="14"/>
         <v>-1724.9000000000233</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G69" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>55</v>
       </c>
@@ -4497,13 +5554,19 @@
         <f t="shared" si="14"/>
         <v>-82077.349999999627</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G70" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="7" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G72" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>0</v>
       </c>
@@ -4516,8 +5579,20 @@
       <c r="D73" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G73" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="H73" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="I73" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="J73" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>24</v>
       </c>
@@ -4533,8 +5608,11 @@
         <f>INDEX(N2:N52,MATCH(A74,A2:A52,0))</f>
         <v>-9181.0800000000163</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G74" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>25</v>
       </c>
@@ -4550,8 +5628,11 @@
         <f t="shared" ref="D75:D79" si="17">INDEX(N3:N53,MATCH(A75,A3:A53,0))</f>
         <v>-311228.08999999997</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G75" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>32</v>
       </c>
@@ -4567,8 +5648,11 @@
         <f t="shared" si="17"/>
         <v>-374962.91000000015</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G76" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>38</v>
       </c>
@@ -4584,8 +5668,11 @@
         <f t="shared" si="17"/>
         <v>-72.879999999888241</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G77" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>39</v>
       </c>
@@ -4601,8 +5688,11 @@
         <f t="shared" si="17"/>
         <v>-1724.9000000000233</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G78" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>55</v>
       </c>
@@ -4618,6 +5708,9 @@
         <f t="shared" si="17"/>
         <v>-82077.349999999627</v>
       </c>
+      <c r="G79" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="7" t="s">
@@ -4631,7 +5724,7 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>71</v>
@@ -4646,11 +5739,11 @@
       </c>
       <c r="B84" s="6">
         <f>INDEX(B$2:B$52,MATCH($A$83,$A$2:$A$52,0))</f>
-        <v>328800</v>
+        <v>24332100</v>
       </c>
       <c r="C84" s="6">
         <f>INDEX(C$2:C$52,MATCH($A$83,$A$2:$A$52,0))</f>
-        <v>321214.59000000003</v>
+        <v>22408587.5499999</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
@@ -4659,11 +5752,11 @@
       </c>
       <c r="B85" s="6">
         <f>INDEX(G$2:G$52,MATCH($A$83,$A$2:$A$52,0))</f>
-        <v>334800</v>
+        <v>24497400</v>
       </c>
       <c r="C85" s="6">
         <f>INDEX(H$2:H$52,MATCH($A$83,$A$2:$A$52,0))</f>
-        <v>312433.70999999897</v>
+        <v>22655993.629999999</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
@@ -4672,11 +5765,11 @@
       </c>
       <c r="B86" s="6">
         <f>INDEX(L$2:L$52,MATCH($A$83,$A$2:$A$52,0))</f>
-        <v>322700</v>
+        <v>24323000</v>
       </c>
       <c r="C86" s="6">
         <f>INDEX(M$2:M$52,MATCH($A$83,$A$2:$A$52,0))</f>
-        <v>322263.03999999998</v>
+        <v>23434073.089999899</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
@@ -4820,6 +5913,8 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B82:B83" xr:uid="{1248789C-8354-428B-8B98-C97B02054C67}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>